<commit_message>
Refactored code. Added comments.
</commit_message>
<xml_diff>
--- a/intrastat/Intrastat Dispatches Data Sample.xlsx
+++ b/intrastat/Intrastat Dispatches Data Sample.xlsx
@@ -451,7 +451,7 @@
         <v>Men's or boys' overcoats</v>
       </c>
       <c r="C2" t="str">
-        <v>0.595</v>
+        <v>595</v>
       </c>
       <c r="D2" t="str">
         <v>190</v>
@@ -492,7 +492,7 @@
         <v>Men's or boys' overcoats</v>
       </c>
       <c r="C3" t="str">
-        <v>0.678</v>
+        <v>678</v>
       </c>
       <c r="D3" t="str">
         <v>150</v>
@@ -533,7 +533,7 @@
         <v>Men's or boys' overcoats</v>
       </c>
       <c r="C4" t="str">
-        <v>0.704</v>
+        <v>704</v>
       </c>
       <c r="D4" t="str">
         <v>175</v>
@@ -574,7 +574,7 @@
         <v>Men's or boys' overcoats</v>
       </c>
       <c r="C5" t="str">
-        <v>0.844</v>
+        <v>844</v>
       </c>
       <c r="D5" t="str">
         <v>135</v>
@@ -615,7 +615,7 @@
         <v>Women's or girls' overcoats</v>
       </c>
       <c r="C6" t="str">
-        <v>0.461</v>
+        <v>461</v>
       </c>
       <c r="D6" t="str">
         <v>145</v>
@@ -656,7 +656,7 @@
         <v>Women's or girls' overcoats</v>
       </c>
       <c r="C7" t="str">
-        <v>0.589</v>
+        <v>589</v>
       </c>
       <c r="D7" t="str">
         <v>160</v>
@@ -697,7 +697,7 @@
         <v>Women's or girls' overcoats</v>
       </c>
       <c r="C8" t="str">
-        <v>0.533</v>
+        <v>533</v>
       </c>
       <c r="D8" t="str">
         <v>155</v>
@@ -738,7 +738,7 @@
         <v>Women's or girls' overcoats</v>
       </c>
       <c r="C9" t="str">
-        <v>0.406</v>
+        <v>406</v>
       </c>
       <c r="D9" t="str">
         <v>180</v>

</xml_diff>